<commit_message>
Implement the new match logic (partially)
</commit_message>
<xml_diff>
--- a/scenarios/cough/processes/Usability1.xlsx
+++ b/scenarios/cough/processes/Usability1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="123">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -346,7 +346,16 @@
     <t xml:space="preserve">[single]</t>
   </si>
   <si>
-    <t xml:space="preserve">GO(match)</t>
+    <t xml:space="preserve">GO(match_decide)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">match_decide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matched = MATCH([api_solver], [water], [swallow], [transport], [fly], [single]), SAVE(matched), IF (ROWS([matched]) == 0) THEN GO(no_match) ELSE GO(match)</t>
   </si>
   <si>
     <t xml:space="preserve">match</t>
@@ -355,13 +364,31 @@
     <t xml:space="preserve">Match</t>
   </si>
   <si>
-    <t xml:space="preserve">Folgende Produkte empfehle ich dir, die zu deinen Anforderungen passen und den Wirkstoff enthalten, für den du dich entschieden hast:</t>
+    <t xml:space="preserve">Folgende Arzneiformen passen optimal zu deinen Bedürfnissen:</t>
   </si>
   <si>
     <t xml:space="preserve">JUMP(Night)</t>
   </si>
   <si>
-    <t xml:space="preserve">MATCH([api_solver], [water], [swallow], [transport], [fly], [single])</t>
+    <t xml:space="preserve">[matched]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no_match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leider gibt es mit dem Wirkstoff/Extrakt {SELECT Name FROM API WHERE ID == [api_solver]},den du ausgewählt hast (show chosen API), keine passenden Medikamente.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeig mir Produkte in der passenden Arzneiformen aber alternativen Wirkstoffen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FINISH()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeig mir Produkte mit dem ausgewählten Wirkstoff aber in einer anderen Arzneiform</t>
   </si>
 </sst>
 </file>
@@ -658,25 +685,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="105" zoomScaleNormal="105" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B26" colorId="64" zoomScale="105" zoomScaleNormal="105" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.39453125" defaultRowHeight="14.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="54.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="53.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.15"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -717,7 +744,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="3" t="s">
@@ -730,7 +757,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="3" t="s">
@@ -743,7 +770,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="28.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
@@ -756,7 +783,7 @@
       </c>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -772,7 +799,7 @@
       </c>
       <c r="F6" s="12"/>
     </row>
-    <row r="7" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7" t="s">
@@ -786,7 +813,7 @@
       </c>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
@@ -800,7 +827,7 @@
       </c>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
@@ -814,7 +841,7 @@
       </c>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
@@ -828,7 +855,7 @@
       </c>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
@@ -842,7 +869,7 @@
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
@@ -856,7 +883,7 @@
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
@@ -870,7 +897,7 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7" t="s">
@@ -884,7 +911,7 @@
       </c>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7" t="s">
@@ -898,7 +925,7 @@
       </c>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="s">
@@ -911,7 +938,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="28.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
         <v>43</v>
       </c>
@@ -928,7 +955,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="28.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
         <v>48</v>
       </c>
@@ -945,7 +972,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="28.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
         <v>52</v>
       </c>
@@ -962,7 +989,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="28.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
         <v>56</v>
       </c>
@@ -979,7 +1006,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="28.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
         <v>60</v>
       </c>
@@ -996,7 +1023,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="28.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
         <v>64</v>
       </c>
@@ -1013,7 +1040,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="28.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
         <v>68</v>
       </c>
@@ -1030,7 +1057,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="28.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
         <v>72</v>
       </c>
@@ -1047,7 +1074,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="28.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
         <v>75</v>
       </c>
@@ -1064,7 +1091,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="28.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
         <v>77</v>
       </c>
@@ -1081,7 +1108,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="28.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>80</v>
       </c>
@@ -1101,7 +1128,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="1" t="s">
         <v>12</v>
       </c>
@@ -1118,7 +1145,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="1" t="s">
         <v>12</v>
       </c>
@@ -1135,7 +1162,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>89</v>
       </c>
@@ -1155,7 +1182,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="1" t="s">
         <v>12</v>
       </c>
@@ -1172,7 +1199,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="1" t="s">
         <v>12</v>
       </c>
@@ -1189,7 +1216,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="28.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>94</v>
       </c>
@@ -1209,7 +1236,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
         <v>12</v>
       </c>
@@ -1226,7 +1253,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="1" t="s">
         <v>12</v>
       </c>
@@ -1243,7 +1270,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>99</v>
       </c>
@@ -1263,7 +1290,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1" t="s">
         <v>12</v>
       </c>
@@ -1280,7 +1307,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1" t="s">
         <v>12</v>
       </c>
@@ -1297,7 +1324,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="28.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>104</v>
       </c>
@@ -1317,7 +1344,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="1" t="s">
         <v>12</v>
       </c>
@@ -1331,7 +1358,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="1" t="s">
         <v>12</v>
       </c>
@@ -1345,26 +1372,74 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="C42" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="E42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F42" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="G42" s="1"/>
+      <c r="D43" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" customFormat="false" ht="41.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>